<commit_message>
VIP and Author แก้ไขข้อมูล และ layour หน้า ConferenceSession
</commit_message>
<xml_diff>
--- a/Conference2018/reports/submission.xlsx
+++ b/Conference2018/reports/submission.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9300" tabRatio="559" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9300" tabRatio="773" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ImportDB-Authors" sheetId="6" r:id="rId4"/>
     <sheet name="gen-qrcode" sheetId="7" r:id="rId5"/>
     <sheet name="VIP" sheetId="8" r:id="rId6"/>
+    <sheet name="ImportToTimeAttendance" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="283">
   <si>
     <t>Computing Theory</t>
   </si>
@@ -863,13 +864,28 @@
   </si>
   <si>
     <t xml:space="preserve"> University North Croatia</t>
+  </si>
+  <si>
+    <t>AttendeeID</t>
+  </si>
+  <si>
+    <t>AttendeeCode</t>
+  </si>
+  <si>
+    <t>Miss Yuka Ueda</t>
+  </si>
+  <si>
+    <t>Mr Duc Hoang Pham</t>
+  </si>
+  <si>
+    <t>info@ahrary.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +917,12 @@
       <sz val="13"/>
       <color rgb="FF333333"/>
       <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -950,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -964,6 +986,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4941,10 +4964,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5046,7 +5069,7 @@
         <v>92</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I44" ca="1" si="0">CONCATENATE("http://www.conference.phuket.psu.ac.th/conference2018/imgs/authors/qrcode/",C3, ".png")</f>
+        <f t="shared" ref="I3:I45" ca="1" si="0">CONCATENATE("http://www.conference.phuket.psu.ac.th/conference2018/imgs/authors/qrcode/",C3, ".png")</f>
         <v>http://www.conference.phuket.psu.ac.th/conference2018/imgs/authors/qrcode/psupic2018126.png</v>
       </c>
     </row>
@@ -6324,7 +6347,66 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="D44" s="7"/>
+      <c r="A44">
+        <v>19</v>
+      </c>
+      <c r="B44">
+        <v>106</v>
+      </c>
+      <c r="C44" t="str">
+        <f ca="1">INDIRECT(ADDRESS(MATCH(D44, 'gen-qrcode'!B:B,0),1,1,,"gen-qrcode"))</f>
+        <v>psupic2018868</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H44" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>http://www.conference.phuket.psu.ac.th/conference2018/imgs/authors/qrcode/psupic2018868.png</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>103</v>
+      </c>
+      <c r="C45" t="str">
+        <f ca="1">INDIRECT(ADDRESS(MATCH(D45, 'gen-qrcode'!B:B,0),1,1,,"gen-qrcode"))</f>
+        <v>psupic2018876</v>
+      </c>
+      <c r="D45" t="s">
+        <v>281</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H45" t="s">
+        <v>95</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>http://www.conference.phuket.psu.ac.th/conference2018/imgs/authors/qrcode/psupic2018876.png</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6334,10 +6416,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7464,7 +7546,7 @@
         <v>65</v>
       </c>
       <c r="E65">
-        <f t="shared" ref="E65:E85" si="3">D65*18</f>
+        <f t="shared" ref="E65:E87" si="3">D65*18</f>
         <v>1170</v>
       </c>
     </row>
@@ -7489,7 +7571,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="str">
-        <f t="shared" ref="A67:A85" si="4">CONCATENATE("psupic2018", LOWER(C67), TEXT(D67, "00"), RIGHT(E67,1))</f>
+        <f t="shared" ref="A67:A87" si="4">CONCATENATE("psupic2018", LOWER(C67), TEXT(D67, "00"), RIGHT(E67,1))</f>
         <v>psupic2018v676</v>
       </c>
       <c r="B67" t="s">
@@ -7846,6 +7928,38 @@
       <c r="E85">
         <f t="shared" si="3"/>
         <v>1530</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="str">
+        <f t="shared" si="4"/>
+        <v>psupic2018868</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D86">
+        <v>86</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="str">
+        <f t="shared" si="4"/>
+        <v>psupic2018876</v>
+      </c>
+      <c r="B87" t="s">
+        <v>281</v>
+      </c>
+      <c r="D87">
+        <v>87</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>1566</v>
       </c>
     </row>
   </sheetData>
@@ -7858,17 +7972,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="145.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="93.42578125" bestFit="1" customWidth="1"/>
@@ -7949,7 +8063,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H48" ca="1" si="0">CONCATENATE("http://www.conference.phuket.psu.ac.th/conference2018/imgs/vips/qrcode/",A3, ".png")</f>
+        <f t="shared" ref="H3:H47" ca="1" si="0">CONCATENATE("http://www.conference.phuket.psu.ac.th/conference2018/imgs/vips/qrcode/",A3, ".png")</f>
         <v>http://www.conference.phuket.psu.ac.th/conference2018/imgs/vips/qrcode/psupic2018g418.png</v>
       </c>
     </row>
@@ -9036,4 +9150,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change psu time attendance service URL
</commit_message>
<xml_diff>
--- a/Conference2018/reports/submission.xlsx
+++ b/Conference2018/reports/submission.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9300" tabRatio="773" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9300" tabRatio="773" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="288">
   <si>
     <t>Computing Theory</t>
   </si>
@@ -881,22 +881,19 @@
     <t>info@ahrary.org</t>
   </si>
   <si>
-    <t>untitleG22</t>
-  </si>
-  <si>
     <t>untitleG23</t>
   </si>
   <si>
     <t>v</t>
   </si>
   <si>
-    <t>psupic2019</t>
-  </si>
-  <si>
-    <t>psupic2020</t>
-  </si>
-  <si>
     <t>กงสุน</t>
+  </si>
+  <si>
+    <t>Consul-General in Phuket, Thailand</t>
+  </si>
+  <si>
+    <t>Mr. Craig Ferguson</t>
   </si>
 </sst>
 </file>
@@ -6437,7 +6434,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7980,16 +7977,16 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" ht="16.5">
       <c r="A88" t="str">
         <f t="shared" si="4"/>
         <v>psupic2018v884</v>
       </c>
-      <c r="B88" t="s">
-        <v>283</v>
+      <c r="B88" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="C88" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D88">
         <v>88</v>
@@ -8005,10 +8002,10 @@
         <v>psupic2018v892</v>
       </c>
       <c r="B89" t="s">
+        <v>283</v>
+      </c>
+      <c r="C89" t="s">
         <v>284</v>
-      </c>
-      <c r="C89" t="s">
-        <v>285</v>
       </c>
       <c r="D89">
         <v>89</v>
@@ -8028,14 +8025,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="62.7109375" customWidth="1"/>
@@ -9202,22 +9199,22 @@
         <v>http://www.conference.phuket.psu.ac.th/conference2018/imgs/vips/qrcode/psupic2018v850.png</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" ht="16.5">
       <c r="A48" t="str">
         <f ca="1">INDIRECT(ADDRESS(MATCH(C48, 'gen-qrcode'!B:B,0),1,1,,"gen-qrcode"))</f>
         <v>psupic2018v884</v>
       </c>
       <c r="B48" t="s">
-        <v>286</v>
-      </c>
-      <c r="C48" t="s">
-        <v>283</v>
+        <v>188</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="D48" t="s">
         <v>265</v>
       </c>
-      <c r="E48" t="s">
-        <v>288</v>
+      <c r="E48" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -9230,16 +9227,16 @@
         <v>psupic2018v892</v>
       </c>
       <c r="B49" t="s">
-        <v>287</v>
+        <v>188</v>
       </c>
       <c r="C49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D49" t="s">
         <v>265</v>
       </c>
       <c r="E49" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -9256,7 +9253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>

</xml_diff>